<commit_message>
Tarea 2 a revision
</commit_message>
<xml_diff>
--- a/kanban.xlsx
+++ b/kanban.xlsx
@@ -208,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,6 +250,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -585,16 +589,16 @@
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="7"/>
@@ -602,14 +606,14 @@
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4"/>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="6"/>

</xml_diff>

<commit_message>
Evito conflicto con archivos Registro.odt y Kanban.slxs
</commit_message>
<xml_diff>
--- a/kanban.xlsx
+++ b/kanban.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Equipo:</t>
   </si>
   <si>
-    <t xml:space="preserve">Alpha</t>
+    <t xml:space="preserve">Delta</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha Inicio:</t>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Proyecto:</t>
   </si>
   <si>
-    <t xml:space="preserve">Tienda Online Prototipo Web</t>
+    <t xml:space="preserve">Proyecto38</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha Fin:</t>
@@ -74,54 +74,19 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">y comprobar que tienen en cuenta las condiciones laborales de los trabajadores de las empresas certificadas. Realizar un documento que determine que certifican estos sellos, como se consiguen, qué garantías dan respecto a los productos certificados. Asignada a Anibal Zambrana</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Tarea 3: Investigar los sellos Textile Exchange </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">y comprobar que tienen en cuenta las condiciones laborales de los trabajadores de las empresas certificadas. Realizar un documento que determine que certifican estos sellos, como se consiguen, qué garantías dan respecto a los productos certificados. Asignada </t>
-    </r>
+    <t xml:space="preserve">Tarea 3: Investigar los sellos Textile Exchange y comprobar que tienen en cuenta las condiciones laborales de los trabajadores de las empresas certificadas. Realizar un documento que determine que certifican estos sellos, como se consiguen, qué garantías dan respecto a los productos certificados. Asignada Erik</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Tarea 4: Investigar el sello Bluesign </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">y comprobar que tienen en cuenta las condiciones laborales de los trabajadores de las empresas certificadas. Realizar un documento que determine que certifican estos sellos, como se consiguen, qué garantías dan respecto a los productos certificados. Asignada a Pablo Guerrero</t>
-    </r>
+    <t xml:space="preserve">Tarea 4: Investigar el sello Bluesign y comprobar que tienen en cuenta las condiciones laborales de los trabajadores de las empresas certificadas. Realizar un documento que determine que certifican estos sellos, como se consiguen, qué garantías dan respecto a los productos certificados. Asignada a Pablo Guerrero</t>
   </si>
   <si>
-    <t xml:space="preserve">Tarea 5: Investigar el indicie de “ buenas practicas en derechos humanos, reciclaje, cuidado del entorno, es decir, en sostenibilidad” encontrado en la  web puntuando en porcentaje a las empresas del sector. Haciendo énfasis en las paginas 44 a 57.</t>
+    <t xml:space="preserve">Tarea 5: Investigar el indicie de “ buenas practicas en derechos humanos, reciclaje, cuidado del entorno, es decir, en sostenibilidad” encontrado en la  web puntuando en porcentaje a las empresas del sector. Haciendo énfasis en las paginas 44 a 57. Asignada a Erik y Angel</t>
   </si>
 </sst>
 </file>
@@ -132,7 +97,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -168,12 +133,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -249,40 +208,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -537,108 +512,108 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="3" t="n">
         <v>45604</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>45613</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1632,7 +1607,7 @@
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="web"/>
+    <hyperlink ref="E10" r:id="rId1" display="Tarea 5: Investigar el indicie de “ buenas practicas en derechos humanos, reciclaje, cuidado del entorno, es decir, en sostenibilidad” encontrado en la  web puntuando en porcentaje a las empresas del sector. Haciendo énfasis en las paginas 44 a 57. Asignada a Erik y Angel"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>